<commit_message>
Nuevas modificaciones y correcciones generales
</commit_message>
<xml_diff>
--- a/public/formats/co-documents-batch.xlsx
+++ b/public/formats/co-documents-batch.xlsx
@@ -7,8 +7,14 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Document" sheetId="1" r:id="rId1"/>
+    <sheet name="Código forma de pago" sheetId="2" r:id="rId2"/>
+    <sheet name="Código metodo de pago" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="CodigoFormaPago">'Código forma de pago'!$B$2:$B$3</definedName>
+    <definedName name="CodigoMetodoPago">'Código metodo de pago'!$B$2:$B$76</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -18,86 +24,792 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>USER</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Numero de factura, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fecha de la factura, dato obligatorio, no puede ser mayor a 10 dias antes de la fecha actual</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Hora de la factura, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Numero de resolucion con la que se va a enviar la factura, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Prefijo de la resolucion de facturacion, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nombre del establecimiento emisor, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Direccion del establecimiento emisor, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Telefono del establecimiento emisor, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Id del municipio del establecimiento, este dato debe consultarlo en la tabla municipios, adjunta en este libro, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Email del establecimiento emisor, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Numero de itentificacion del cliente, dato obligatorio, el cliente ya debe existir en la base de datos.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Id de la forma de pago de la factura, puede seleccionar una opcion de la lista o escribir el codigo correspondiente de la tabla anexa formas de pago, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Id del metodo de pago de la factura, puede seleccionar una opcion de la lista o escribir el codigo correspondiente de la tabla anexa metodos de pago, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Fecha de vencimiento de la factura, debe corresponder a la fecha de la factura + plazo en dias, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Plazo en dias de la factura, para facturas de contado colocar cero, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Total Valor Bruto antes de tributos, suma de los valores brutos de las líneas de la factura, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Total Valor Base Imponible, Base imponible para el cálculo de los tributos, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Total valor bruto mas impuestos, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Total descuentos de la factura, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Total cargos de la factura, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Valor total de la factura con descuentos y cargos, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cantidad facturada de la linea de detalle, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Valor Base Imponible de la linea de detalle, Base imponible para el cálculo de los tributos, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Referencia del articulo de la linea de detalle, el articulo debe existir en la base de datos, dato obligatorio.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Precio de venta al publico del producto o servicio, incluye impuestos, dato obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Informacion que saldra en la cabecera de la factura</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Informacion que saldra en el pie de pagina de la factura</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Notas de la factura, se incluye en el XML en el campo correspondiente &lt;cbc:note&gt;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dato obligatorio para facturas del sector salud, opcional para facturas estándar, indica el inicio del periodo de facturacion.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dato obligatorio para facturas del sector salud, opcional para facturas estándar, indica el final del periodo de facturacion.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">USER:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+La informacion contenida en esta columna es opcional, debe incluirse si es una factura del sector salud y obedece al siguiente formato:
+- Cada campo debe separarse por comas ,
+- Para facturas multiusuario, cada registro se separa por %
+- Cuando un campo tenga varios valores como por ejemplo el campo numeros de autorizacion, estos deben estar separados por punto y coma ;
+- Cuando un campo no necesite incluirse en un registro, por ejemplo cuando un usuario no tiene segundo nombre, se debe colocar dos comas ,,
+- El orden de cada campo es el siguiente:
+     codigo_proveedor,id_tipo_documento_identificacion,numero_documento,apellido,segundo_apellido,primer_nombre,segundo_nombre,id_tipo_usuario_salud,
+     id_metodo_pago_contrato_salud,id_cobertura_salud,numeros_autorizacion,mipres,entrega_mipres,numero_contrato,numero_poliza,co_pago,
+     cuota_moderadora,cuota_recuperacion,pago_compartido
+En el ejemplo del archivo, cada dato corresponde de la siguiente manera:
+                "codigo_proveedor": "AF-0000500-85-XX-001",
+                "id_tipo_documento_identificacion": 4,
+                "numero_documento": "A89008003",
+                "apellido": "OBANDO",
+                "segundo_apellido": "LONDOÑO",
+                "primer_nombre": "ALEXANDER",
+                "segundo_nombre": "",
+                "id_tipo_usuario_salud": 1,
+                "id_metodo_pago_contrato_salud": 7,
+                "id_cobertura_salud": 5,
+                "numeros_autorizacion": "A12345;604567;AX-2345",
+                "mipres": "RNA3D345;664FF04567;ARXXX-2765345",
+                "entrega_mipres": "RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345",
+                "numero_contrato": "1000-2021-0005698",
+                "numero_poliza": "1045-2FG01-0567228",
+                "co_pago": "3300.00",
+                "cuota_moderadora": "5800.00",
+                "cuota_recuperacion": "105000.00",
+                "pago_compartido": "225000.00"
+Los campos que tengan id como por ejemplo: id_cobertura_salud, tienen sus posibles valores y significados en las tablas adjuntas</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="53">
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>resolution_number</t>
-  </si>
-  <si>
-    <t>prefix</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>establishment_name</t>
-  </si>
-  <si>
-    <t>establishment_address</t>
-  </si>
-  <si>
-    <t>establishment_phone</t>
-  </si>
-  <si>
-    <t>establishment_municipality</t>
-  </si>
-  <si>
-    <t>establishment_email</t>
-  </si>
-  <si>
-    <t>payment_form_id</t>
-  </si>
-  <si>
-    <t>payment_method_id</t>
-  </si>
-  <si>
-    <t>payment_due_date</t>
-  </si>
-  <si>
-    <t>duration_measure</t>
-  </si>
-  <si>
-    <t>line_extension_amount</t>
-  </si>
-  <si>
-    <t>tax_exclusive_amount</t>
-  </si>
-  <si>
-    <t>tax_inclusive_amount</t>
-  </si>
-  <si>
-    <t>allowance_total_amount</t>
-  </si>
-  <si>
-    <t>charge_total_amount</t>
-  </si>
-  <si>
-    <t>payable_amount</t>
-  </si>
-  <si>
-    <t>invoiced_quantity</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>price_amount</t>
-  </si>
-  <si>
-    <t>head_note</t>
-  </si>
-  <si>
-    <t>foot_note</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="131">
   <si>
     <t>Periodo facturacion Junio 2023</t>
   </si>
@@ -129,9 +841,6 @@
     <t>SETP</t>
   </si>
   <si>
-    <t>customer</t>
-  </si>
-  <si>
     <t>PRUEBA1</t>
   </si>
   <si>
@@ -144,15 +853,6 @@
     <t>300000.00</t>
   </si>
   <si>
-    <t>invoice_period_start_date</t>
-  </si>
-  <si>
-    <t>invoice_period_end_date</t>
-  </si>
-  <si>
-    <t>users_info</t>
-  </si>
-  <si>
     <t>AF-0000500-85-XX-001,4,A89008003,OBANDO,LONDOÑO,ALEXANDER,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
   </si>
   <si>
@@ -162,22 +862,346 @@
     <t>AF-0000500-85-XX-001,4,A89008003,OBANDO,LONDOÑO,ALEXANDER,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00%AF-0000500-85-XX-001,4,A41946692,CARDONA,VILLADA,ELIZABETH,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
   </si>
   <si>
-    <t>991500164</t>
-  </si>
-  <si>
-    <t>991500165</t>
-  </si>
-  <si>
-    <t>991500166</t>
-  </si>
-  <si>
-    <t>991500167</t>
-  </si>
-  <si>
-    <t>991500168</t>
-  </si>
-  <si>
-    <t>991500169</t>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>numero_resolucion</t>
+  </si>
+  <si>
+    <t>prefijo</t>
+  </si>
+  <si>
+    <t>nombre_establecimiento</t>
+  </si>
+  <si>
+    <t>direccion_establecimiento</t>
+  </si>
+  <si>
+    <t>telefono_establecimiento</t>
+  </si>
+  <si>
+    <t>municipio_establecimiento</t>
+  </si>
+  <si>
+    <t>email_establecimiento</t>
+  </si>
+  <si>
+    <t>idetificacion_cliente</t>
+  </si>
+  <si>
+    <t>id_forma_pago</t>
+  </si>
+  <si>
+    <t>id_metodo_pago</t>
+  </si>
+  <si>
+    <t>fecha_vencimiento</t>
+  </si>
+  <si>
+    <t>plazo_dias</t>
+  </si>
+  <si>
+    <t>total_impuestos_incl</t>
+  </si>
+  <si>
+    <t>total_descuentos</t>
+  </si>
+  <si>
+    <t>total_cargos</t>
+  </si>
+  <si>
+    <t>total_pagado</t>
+  </si>
+  <si>
+    <t>cantidad_linea</t>
+  </si>
+  <si>
+    <t>base_impuestos_linea</t>
+  </si>
+  <si>
+    <t>codigo_linea</t>
+  </si>
+  <si>
+    <t>precio_venta</t>
+  </si>
+  <si>
+    <t>nota_cabecera</t>
+  </si>
+  <si>
+    <t>nota_pie</t>
+  </si>
+  <si>
+    <t>notas_factura</t>
+  </si>
+  <si>
+    <t>fecha_inicial_perido_facturado</t>
+  </si>
+  <si>
+    <t>fecha_final_perido_facturado</t>
+  </si>
+  <si>
+    <t>informacion_usuarios_sector_salud</t>
+  </si>
+  <si>
+    <t>total_base_impuestos</t>
+  </si>
+  <si>
+    <t>total_valor_bruto</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Contado</t>
+  </si>
+  <si>
+    <t>Crédito</t>
+  </si>
+  <si>
+    <t>Instrumento no definido</t>
+  </si>
+  <si>
+    <t>Crédito ACH</t>
+  </si>
+  <si>
+    <t>Débito ACH</t>
+  </si>
+  <si>
+    <t>Reversión débito de demanda ACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversión crédito de demanda ACH </t>
+  </si>
+  <si>
+    <t>Crédito de demanda ACH</t>
+  </si>
+  <si>
+    <t>Débito de demanda ACH</t>
+  </si>
+  <si>
+    <t>Mantener</t>
+  </si>
+  <si>
+    <t>Clearing Nacional o Regional</t>
+  </si>
+  <si>
+    <t>Efectivo</t>
+  </si>
+  <si>
+    <t>Reversión Crédito Ahorro</t>
+  </si>
+  <si>
+    <t>Reversión Débito Ahorro</t>
+  </si>
+  <si>
+    <t>Crédito Ahorro</t>
+  </si>
+  <si>
+    <t>Débito Ahorro</t>
+  </si>
+  <si>
+    <t>Bookentry Crédito</t>
+  </si>
+  <si>
+    <t>Bookentry Débito</t>
+  </si>
+  <si>
+    <t>Concentración de la demanda en efectivo /Desembolso Crédito (CCD)</t>
+  </si>
+  <si>
+    <t>Concentración de la demanda en efectivo / Desembolso (CCD) débito</t>
+  </si>
+  <si>
+    <t>Crédito Pago negocio corporativo (CTP)</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>Poyecto bancario</t>
+  </si>
+  <si>
+    <t>Proyecto bancario certificado</t>
+  </si>
+  <si>
+    <t>Cheque bancario</t>
+  </si>
+  <si>
+    <t>Nota cambiaria esperando aceptación</t>
+  </si>
+  <si>
+    <t>Cheque certificado</t>
+  </si>
+  <si>
+    <t>Cheque Local</t>
+  </si>
+  <si>
+    <t>Débito Pago Neogcio Corporativo (CTP)</t>
+  </si>
+  <si>
+    <t>Crédito Negocio Intercambio Corporativo (CTX)</t>
+  </si>
+  <si>
+    <t>Débito Negocio Intercambio Corporativo (CTX)</t>
+  </si>
+  <si>
+    <t>Transferecia Crédito</t>
+  </si>
+  <si>
+    <t>Transferencia Débito</t>
+  </si>
+  <si>
+    <t>Concentración Efectivo / Desembolso Crédito plus (CCD+)</t>
+  </si>
+  <si>
+    <t>Concentración Efectivo / Desembolso Débito plus (CCD+)</t>
+  </si>
+  <si>
+    <t>Pago y depósito pre acordado (PPD)</t>
+  </si>
+  <si>
+    <t>Concentración efectivo ahorros / Desembolso Crédito (CCD)</t>
+  </si>
+  <si>
+    <t>Concentración efectivo ahorros / Desembolso Drédito (CCD)</t>
+  </si>
+  <si>
+    <t>Pago Negocio Corporativo Ahorros Crédito (CTP)</t>
+  </si>
+  <si>
+    <t>Pago Neogcio Corporativo Ahorros Débito (CTP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentración efectivo/Desembolso Crédito plus (CCD+) </t>
+  </si>
+  <si>
+    <t>Consiganción bancaria</t>
+  </si>
+  <si>
+    <t>Concentración efectivo / Desembolso Débito plus (CCD+)</t>
+  </si>
+  <si>
+    <t>Nota cambiaria</t>
+  </si>
+  <si>
+    <t>Transferencia Crédito Bancario</t>
+  </si>
+  <si>
+    <t>Transferencia Débito Interbancario</t>
+  </si>
+  <si>
+    <t>Transferencia Débito Bancaria</t>
+  </si>
+  <si>
+    <t>Tarjeta Crédito</t>
+  </si>
+  <si>
+    <t>Tarjeta Débito</t>
+  </si>
+  <si>
+    <t>Postgiro</t>
+  </si>
+  <si>
+    <t>Telex estándar bancario francés</t>
+  </si>
+  <si>
+    <t>Pago comercial urgente</t>
+  </si>
+  <si>
+    <t>Pago Tesorería Urgente</t>
+  </si>
+  <si>
+    <t>Nota promisoria</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por el acreedor</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por el acreedor, avalada por el banco</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por el acreedor, avalada por un tercero</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada pro el banco</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por un banco avalada por otro banco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nota promisoria firmada </t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por un tercero avalada por un banco</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el por el acreedor</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el por el acreedor sobre un banco</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el acreedor, avalada por otro banco</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el acreedor, sobre un banco avalada por un tercero</t>
+  </si>
+  <si>
+    <t>Retiro de una nota por el acreedor sobre un tercero</t>
+  </si>
+  <si>
+    <t>Retiro de una nota por el acreedor sobre un tercero avalada por un banco</t>
+  </si>
+  <si>
+    <t>Nota bancaria tranferible</t>
+  </si>
+  <si>
+    <t>Cheque local traferible</t>
+  </si>
+  <si>
+    <t>Giro referenciado</t>
+  </si>
+  <si>
+    <t>Giro urgente</t>
+  </si>
+  <si>
+    <t>Giro formato abierto</t>
+  </si>
+  <si>
+    <t>Método de pago solicitado no usuado</t>
+  </si>
+  <si>
+    <t>Clearing entre partners</t>
+  </si>
+  <si>
+    <t>Acuerdo mutuo</t>
+  </si>
+  <si>
+    <t>991500178</t>
+  </si>
+  <si>
+    <t>991500179</t>
+  </si>
+  <si>
+    <t>991500180</t>
+  </si>
+  <si>
+    <t>991500181</t>
+  </si>
+  <si>
+    <t>991500182</t>
+  </si>
+  <si>
+    <t>991500183</t>
   </si>
 </sst>
 </file>
@@ -188,7 +1212,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +1225,19 @@
       <color rgb="FF212529"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -511,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -523,13 +1560,13 @@
     <col min="4" max="4" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -540,132 +1577,132 @@
     <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="94.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="244.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U1" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
       <c r="W1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="AB1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="AC1" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AD1" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AE1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:31">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="B2" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C2" s="4">
         <v>0.69513888888888886</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H2">
         <v>3899301</v>
@@ -674,61 +1711,61 @@
         <v>1006</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K2">
         <v>89008003</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>47</v>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" t="s">
+        <v>52</v>
       </c>
       <c r="N2" s="3">
-        <v>45169</v>
+        <v>45210</v>
       </c>
       <c r="O2">
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Q2" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T2" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="V2">
         <v>1</v>
       </c>
       <c r="W2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X2" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="Y2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z2" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB2" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="3">
         <v>45108</v>
@@ -737,30 +1774,30 @@
         <v>45138</v>
       </c>
       <c r="AE2" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="B3" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C3" s="4">
         <v>0.6958333333333333</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H3">
         <v>3899301</v>
@@ -769,61 +1806,61 @@
         <v>1006</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K3">
         <v>89008003</v>
       </c>
-      <c r="L3">
-        <v>1</v>
+      <c r="L3" t="s">
+        <v>50</v>
       </c>
       <c r="M3">
         <v>47</v>
       </c>
       <c r="N3" s="3">
-        <v>45169</v>
+        <v>45180</v>
       </c>
       <c r="O3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T3" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X3" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="Y3" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z3" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA3" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB3" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="3">
         <v>45108</v>
@@ -832,30 +1869,30 @@
         <v>45138</v>
       </c>
       <c r="AE3" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:31">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="B4" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C4" s="4">
         <v>0.69652777777777775</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H4">
         <v>3899301</v>
@@ -864,84 +1901,84 @@
         <v>1006</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <v>89008003</v>
       </c>
       <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>47</v>
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>57</v>
       </c>
       <c r="N4" s="3">
-        <v>45169</v>
+        <v>45210</v>
       </c>
       <c r="O4">
         <v>30</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="Q4" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R4" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T4" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U4" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="V4">
         <v>1</v>
       </c>
       <c r="W4" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="Y4" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z4" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA4" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB4" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="B5" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C5" s="4">
         <v>0.6972222222222223</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H5">
         <v>3899301</v>
@@ -950,61 +1987,61 @@
         <v>1006</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>89008003</v>
       </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <v>47</v>
       </c>
       <c r="N5" s="3">
-        <v>45169</v>
+        <v>45210</v>
       </c>
       <c r="O5">
         <v>30</v>
       </c>
       <c r="P5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="S5" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T5" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="V5">
         <v>1</v>
       </c>
       <c r="W5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X5" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="Y5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z5" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA5" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB5" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="3">
         <v>45108</v>
@@ -1013,30 +2050,30 @@
         <v>45138</v>
       </c>
       <c r="AE5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C6" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H6">
         <v>3899301</v>
@@ -1045,61 +2082,61 @@
         <v>1006</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <v>89008003</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M6">
         <v>47</v>
       </c>
       <c r="N6" s="3">
-        <v>45169</v>
+        <v>45210</v>
       </c>
       <c r="O6">
         <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="Q6" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R6" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="S6" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T6" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U6" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="V6">
         <v>1</v>
       </c>
       <c r="W6" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X6" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="Y6" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z6" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA6" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB6" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="3">
         <v>45108</v>
@@ -1110,25 +2147,25 @@
     </row>
     <row r="7" spans="1:31">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C7" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H7">
         <v>3899301</v>
@@ -1137,61 +2174,61 @@
         <v>1006</v>
       </c>
       <c r="J7" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K7">
         <v>89008003</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7">
         <v>47</v>
       </c>
       <c r="N7" s="3">
-        <v>45169</v>
+        <v>45210</v>
       </c>
       <c r="O7">
         <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="Q7" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="S7" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T7" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U7" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="V7">
         <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="Y7" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z7" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA7" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB7" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="3">
         <v>45108</v>
@@ -1202,25 +2239,25 @@
     </row>
     <row r="8" spans="1:31">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B8" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C8" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H8">
         <v>3899301</v>
@@ -1229,61 +2266,61 @@
         <v>1006</v>
       </c>
       <c r="J8" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <v>89008003</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M8">
         <v>47</v>
       </c>
       <c r="N8" s="3">
-        <v>45169</v>
+        <v>45210</v>
       </c>
       <c r="O8">
         <v>30</v>
       </c>
       <c r="P8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="Q8" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="S8" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T8" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U8" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="V8">
         <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X8" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="Y8" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z8" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA8" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB8" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="3">
         <v>45108</v>
@@ -1294,25 +2331,25 @@
     </row>
     <row r="9" spans="1:31">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="B9" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C9" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H9">
         <v>3899301</v>
@@ -1321,61 +2358,61 @@
         <v>1006</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K9">
         <v>89008003</v>
       </c>
-      <c r="L9">
-        <v>1</v>
+      <c r="L9" t="s">
+        <v>50</v>
       </c>
       <c r="M9">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="N9" s="3">
-        <v>45169</v>
+        <v>45180</v>
       </c>
       <c r="O9">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="Q9" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R9" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="S9" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T9" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U9" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="V9">
         <v>1</v>
       </c>
       <c r="W9" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X9" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="Y9" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z9" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA9" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB9" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="3">
         <v>45108</v>
@@ -1384,30 +2421,30 @@
         <v>45138</v>
       </c>
       <c r="AE9" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="B10" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C10" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H10">
         <v>3899301</v>
@@ -1416,61 +2453,61 @@
         <v>1006</v>
       </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <v>89008003</v>
       </c>
-      <c r="L10">
-        <v>1</v>
+      <c r="L10" t="s">
+        <v>50</v>
       </c>
       <c r="M10">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="N10" s="3">
-        <v>45169</v>
+        <v>45180</v>
       </c>
       <c r="O10">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="Q10" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R10" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="S10" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T10" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U10" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="V10">
         <v>1</v>
       </c>
       <c r="W10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X10" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="Y10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z10" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA10" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB10" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC10" s="3">
         <v>45108</v>
@@ -1479,30 +2516,30 @@
         <v>45138</v>
       </c>
       <c r="AE10" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="2" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="B11" s="3">
-        <v>45138</v>
+        <v>45180</v>
       </c>
       <c r="C11" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="H11">
         <v>3899301</v>
@@ -1511,61 +2548,61 @@
         <v>1006</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <v>89008003</v>
       </c>
-      <c r="L11">
-        <v>1</v>
+      <c r="L11" t="s">
+        <v>50</v>
       </c>
       <c r="M11">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="N11" s="3">
-        <v>45169</v>
+        <v>45180</v>
       </c>
       <c r="O11">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="Q11" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="R11" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="S11" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="T11" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="U11" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="V11">
         <v>1</v>
       </c>
       <c r="W11" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="X11" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="Y11" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="Z11" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="AA11" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="AB11" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="3">
         <v>45108</v>
@@ -1574,11 +2611,690 @@
         <v>45138</v>
       </c>
       <c r="AE11" t="s">
-        <v>46</v>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="L2:L11">
+      <formula1>CodigoFormaPago</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="M2:M11">
+      <formula1>CodigoMetodoPago</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>